<commit_message>
Working on inventory and cleaning up the tests structure
</commit_message>
<xml_diff>
--- a/testing/TestBookKeeping_20180502.xlsx
+++ b/testing/TestBookKeeping_20180502.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaestner/git/imagingsuite/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A72D4342-41F5-4547-82DE-FEC031707907}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F36EF6FE-132A-3C4A-AD3E-8F6C7915B2A4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18220" yWindow="7400" windowWidth="28040" windowHeight="17440" xr2:uid="{5DD009DC-2437-E84C-883A-EAE52A5B12F3}"/>
+    <workbookView xWindow="15040" yWindow="3480" windowWidth="28040" windowHeight="17440" xr2:uid="{5DD009DC-2437-E84C-883A-EAE52A5B12F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="files" localSheetId="0">Sheet1!$A$2:$A$499</definedName>
+    <definedName name="files" localSheetId="0">Sheet1!$A$2:$A$474</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,8 +29,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{DC063405-1B17-EE43-AFBB-8DAF172661D3}" name="files" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/kaestner/git/imagingsuite/testing/files.log" thousands="'">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="files" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="/Users/kaestner/git/imagingsuite/testing/files.log" thousands="'">
       <textFields>
         <textField/>
       </textFields>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="472">
   <si>
     <t>./applications/imageviewer/imageviewer/saveasdialog.h</t>
   </si>
@@ -180,45 +180,12 @@
     <t>./core/kipl/kipl/include/base/core/imagearithmetics.h</t>
   </si>
   <si>
-    <t>./core/kipl/kipl/include/base/core/imagecast.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/base/core/imagesamplers.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/base/core/marginsetter.hpp</t>
-  </si>
-  <si>
     <t>./core/kipl/kipl/include/base/core/quad.h</t>
   </si>
   <si>
     <t>./core/kipl/kipl/include/base/core/sharedbuffer.h</t>
   </si>
   <si>
-    <t>./core/kipl/kipl/include/base/core/textractor.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/base/core/thistogram.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/base/core/timage.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/base/core/tpermuteimage.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/base/core/tprofile.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/base/core/transpose.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/base/core/trotate.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/base/core/tsubimage.hpp</t>
-  </si>
-  <si>
     <t>./core/kipl/kipl/include/base/imagecast.h</t>
   </si>
   <si>
@@ -420,36 +387,6 @@
     <t>./core/kipl/kipl/include/math/compleximage.h</t>
   </si>
   <si>
-    <t>./core/kipl/kipl/include/math/core/basicprojector.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/math/core/compleximage.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/math/core/covariance.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/math/core/image_statistics.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/math/core/LinearAlgebra.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/math/core/linfit.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/math/core/mathfunctions.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/math/core/median.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/math/core/statistics.hpp</t>
-  </si>
-  <si>
-    <t>./core/kipl/kipl/include/math/core/tcenterofgravity.hpp</t>
-  </si>
-  <si>
     <t>./core/kipl/kipl/include/math/covariance.h</t>
   </si>
   <si>
@@ -777,12 +714,6 @@
     <t>./core/kipl/kipl/include/wavelets/wavelets.h</t>
   </si>
   <si>
-    <t>./core/kipl/UnitTests/KiplTests/tstcovariance.h</t>
-  </si>
-  <si>
-    <t>./core/kipl/UnitTests/KiplTests/tstDirAnalyzer.h</t>
-  </si>
-  <si>
     <t>./core/modules/ModuleConfig/include/ConfigBase.h</t>
   </si>
   <si>
@@ -1459,6 +1390,72 @@
   </si>
   <si>
     <t>TestProject</t>
+  </si>
+  <si>
+    <t>tDirAnalysis</t>
+  </si>
+  <si>
+    <t>tImageOperators</t>
+  </si>
+  <si>
+    <t>tIndex2Coord</t>
+  </si>
+  <si>
+    <t>tKIPL_IO</t>
+  </si>
+  <si>
+    <t>tKiplAdvFilters</t>
+  </si>
+  <si>
+    <t>Development framework</t>
+  </si>
+  <si>
+    <t>tkiplbasetest</t>
+  </si>
+  <si>
+    <t>tKIPLbaseTImage</t>
+  </si>
+  <si>
+    <t>tkipliotest</t>
+  </si>
+  <si>
+    <t>tKiplMath</t>
+  </si>
+  <si>
+    <t>Not really a test, but development framework</t>
+  </si>
+  <si>
+    <t>Only tests the sign function</t>
+  </si>
+  <si>
+    <t>tkiplmorphologytest</t>
+  </si>
+  <si>
+    <t>FillHole, tkiplmorphologytest</t>
+  </si>
+  <si>
+    <t>Empty test project, hMax workbench</t>
+  </si>
+  <si>
+    <t>tKIPLStrings</t>
+  </si>
+  <si>
+    <t>tLinFit</t>
+  </si>
+  <si>
+    <t>Single good test case</t>
+  </si>
+  <si>
+    <t>tNoiseImage</t>
+  </si>
+  <si>
+    <t>tModuleConfig</t>
+  </si>
+  <si>
+    <t>Very basic tests</t>
+  </si>
+  <si>
+    <t>basic read write</t>
   </si>
 </sst>
 </file>
@@ -1515,7 +1512,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="files" connectionId="1" xr16:uid="{AD842ACF-C860-FD46-AD20-0C7E6A92B2EC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="files" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1815,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8DFD1B-7415-AE4F-A94D-DB41DC7D4765}">
-  <dimension ref="A1:E499"/>
+  <dimension ref="A1:E474"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="E117" sqref="E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1831,19 +1828,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>467</v>
+        <v>444</v>
       </c>
       <c r="B1" t="s">
-        <v>468</v>
+        <v>445</v>
       </c>
       <c r="C1" t="s">
-        <v>472</v>
+        <v>449</v>
       </c>
       <c r="D1" t="s">
-        <v>469</v>
+        <v>446</v>
       </c>
       <c r="E1" t="s">
-        <v>470</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1851,7 +1848,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>471</v>
+        <v>448</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -1862,7 +1859,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>471</v>
+        <v>448</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -1873,7 +1870,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>471</v>
+        <v>448</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -2220,9 +2217,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D51" s="1">
-        <v>0</v>
-      </c>
+      <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
@@ -2252,8 +2247,11 @@
       <c r="A55" t="s">
         <v>47</v>
       </c>
+      <c r="C55" t="s">
+        <v>457</v>
+      </c>
       <c r="D55" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -2268,16 +2266,22 @@
       <c r="A57" t="s">
         <v>49</v>
       </c>
+      <c r="C57" t="s">
+        <v>456</v>
+      </c>
       <c r="D57" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>50</v>
       </c>
+      <c r="C58" t="s">
+        <v>451</v>
+      </c>
       <c r="D58" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -2292,8 +2296,11 @@
       <c r="A60" t="s">
         <v>52</v>
       </c>
+      <c r="C60" t="s">
+        <v>452</v>
+      </c>
       <c r="D60" s="1">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -2316,8 +2323,11 @@
       <c r="A63" t="s">
         <v>55</v>
       </c>
+      <c r="C63" t="s">
+        <v>456</v>
+      </c>
       <c r="D63" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -2340,16 +2350,22 @@
       <c r="A66" t="s">
         <v>58</v>
       </c>
+      <c r="C66" t="s">
+        <v>456</v>
+      </c>
       <c r="D66" s="1">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>59</v>
       </c>
+      <c r="C67" t="s">
+        <v>457</v>
+      </c>
       <c r="D67" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2380,29 +2396,30 @@
       <c r="A71" t="s">
         <v>63</v>
       </c>
+      <c r="C71" t="s">
+        <v>456</v>
+      </c>
       <c r="D71" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>64</v>
       </c>
+      <c r="C72" t="s">
+        <v>456</v>
+      </c>
       <c r="D72" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>65</v>
-      </c>
-      <c r="D73" s="1">
-        <v>0</v>
-      </c>
+      <c r="D73" s="1"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D74" s="1">
         <v>0</v>
@@ -2410,7 +2427,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D75" s="1">
         <v>0</v>
@@ -2418,23 +2435,20 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D76" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>69</v>
-      </c>
       <c r="D77" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D78" s="1">
         <v>0</v>
@@ -2442,23 +2456,20 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D79" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>72</v>
-      </c>
       <c r="D80" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D81" s="1">
         <v>0</v>
@@ -2466,7 +2477,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D82" s="1">
         <v>0</v>
@@ -2474,7 +2485,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D83" s="1">
         <v>0</v>
@@ -2487,7 +2498,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D85" s="1">
         <v>0</v>
@@ -2495,7 +2506,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D86" s="1">
         <v>0</v>
@@ -2503,20 +2514,23 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D87" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>76</v>
+      </c>
       <c r="D88" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D89" s="1">
         <v>0</v>
@@ -2524,20 +2538,23 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D90" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>79</v>
+      </c>
       <c r="D91" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D92" s="1">
         <v>0</v>
@@ -2545,7 +2562,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D93" s="1">
         <v>0</v>
@@ -2553,13 +2570,16 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>82</v>
+      </c>
+      <c r="D94" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>83</v>
       </c>
-      <c r="D94" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D95" s="1">
         <v>0</v>
       </c>
@@ -2572,15 +2592,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>85</v>
       </c>
+      <c r="C97" t="s">
+        <v>454</v>
+      </c>
       <c r="D97" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.2</v>
+      </c>
+      <c r="E97" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>86</v>
       </c>
@@ -2588,7 +2614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>87</v>
       </c>
@@ -2596,174 +2622,192 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>88</v>
       </c>
-      <c r="D100" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+      <c r="D101" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
         <v>89</v>
       </c>
-      <c r="D101" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+      <c r="C102" t="s">
+        <v>468</v>
+      </c>
+      <c r="D102" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E102" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>90</v>
       </c>
-      <c r="D102" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="D103" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>91</v>
       </c>
-      <c r="D103" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="D104" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>92</v>
       </c>
-      <c r="D104" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="D105" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>93</v>
       </c>
-      <c r="D105" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+      <c r="D106" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>94</v>
       </c>
-      <c r="D106" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="D107" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D108" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>95</v>
       </c>
-      <c r="D107" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="D109" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D110" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>96</v>
       </c>
-      <c r="D108" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+      <c r="D111" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>97</v>
       </c>
-      <c r="D109" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+      <c r="C112" t="s">
+        <v>458</v>
+      </c>
+      <c r="D112" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>98</v>
       </c>
-      <c r="D110" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D111" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+      <c r="D113" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
         <v>99</v>
       </c>
-      <c r="D112" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+      <c r="D114" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
         <v>100</v>
       </c>
-      <c r="D113" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+      <c r="C115" t="s">
+        <v>450</v>
+      </c>
+      <c r="D115" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>101</v>
       </c>
-      <c r="D114" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+      <c r="C116" t="s">
+        <v>458</v>
+      </c>
+      <c r="D116" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E116" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
         <v>102</v>
       </c>
-      <c r="D115" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+      <c r="D117" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>103</v>
       </c>
-      <c r="D116" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+      <c r="D118" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
         <v>104</v>
       </c>
-      <c r="D117" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+      <c r="D119" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
         <v>105</v>
       </c>
-      <c r="D118" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D119" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+      <c r="D120" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
         <v>106</v>
       </c>
-      <c r="D120" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D121" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>107</v>
       </c>
@@ -2771,23 +2815,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>108</v>
       </c>
+      <c r="C123" t="s">
+        <v>453</v>
+      </c>
       <c r="D123" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>109</v>
       </c>
+      <c r="C124" t="s">
+        <v>458</v>
+      </c>
       <c r="D124" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>110</v>
       </c>
@@ -2795,113 +2845,125 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D126" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
         <v>111</v>
       </c>
-      <c r="D126" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
+      <c r="D127" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D128" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
         <v>112</v>
       </c>
-      <c r="D127" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
+      <c r="D129" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>113</v>
       </c>
-      <c r="D128" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
+      <c r="C130" t="s">
+        <v>459</v>
+      </c>
+      <c r="D130" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E130" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
         <v>114</v>
       </c>
-      <c r="D129" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
+      <c r="D131" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
         <v>115</v>
       </c>
-      <c r="D130" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
+      <c r="D132" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
         <v>116</v>
       </c>
-      <c r="D131" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
+      <c r="D133" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>117</v>
       </c>
-      <c r="D132" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
+      <c r="D134" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>118</v>
       </c>
-      <c r="D133" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
+      <c r="D135" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
         <v>119</v>
       </c>
-      <c r="D134" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
+      <c r="D136" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
         <v>120</v>
       </c>
-      <c r="D135" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
+      <c r="C137" t="s">
+        <v>466</v>
+      </c>
+      <c r="D137" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="E137" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
         <v>121</v>
       </c>
-      <c r="D136" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D137" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
+      <c r="D138" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
         <v>122</v>
       </c>
-      <c r="D138" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D139" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>123</v>
       </c>
@@ -2909,15 +2971,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>124</v>
       </c>
+      <c r="C141" t="s">
+        <v>459</v>
+      </c>
       <c r="D141" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.1</v>
+      </c>
+      <c r="E141" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>125</v>
       </c>
@@ -2925,7 +2993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>126</v>
       </c>
@@ -2933,7 +3001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>127</v>
       </c>
@@ -2941,7 +3009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>128</v>
       </c>
@@ -2949,15 +3017,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>129</v>
       </c>
+      <c r="C146" t="s">
+        <v>459</v>
+      </c>
       <c r="D146" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>130</v>
       </c>
@@ -2965,15 +3036,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>131</v>
       </c>
+      <c r="C148" t="s">
+        <v>459</v>
+      </c>
       <c r="D148" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>132</v>
       </c>
@@ -2981,89 +3055,95 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D150" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
         <v>133</v>
       </c>
-      <c r="D150" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
+      <c r="D151" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
         <v>134</v>
       </c>
-      <c r="D151" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
+      <c r="D152" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>135</v>
       </c>
-      <c r="D152" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
+      <c r="D153" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
         <v>136</v>
       </c>
-      <c r="D153" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
+      <c r="D154" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
         <v>137</v>
       </c>
-      <c r="D154" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
+      <c r="D155" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
         <v>138</v>
       </c>
-      <c r="D155" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
+      <c r="D156" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
         <v>139</v>
       </c>
-      <c r="D156" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
+      <c r="D157" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
         <v>140</v>
       </c>
-      <c r="D157" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
+      <c r="C158" t="s">
+        <v>463</v>
+      </c>
+      <c r="D158" s="1">
+        <v>0</v>
+      </c>
+      <c r="E158" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
         <v>141</v>
       </c>
-      <c r="D158" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
+      <c r="C159" t="s">
+        <v>462</v>
+      </c>
+      <c r="D159" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
         <v>142</v>
-      </c>
-      <c r="D159" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
-        <v>143</v>
       </c>
       <c r="D160" s="1">
         <v>0</v>
@@ -3071,7 +3151,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D161" s="1">
         <v>0</v>
@@ -3079,7 +3159,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D162" s="1">
         <v>0</v>
@@ -3087,7 +3167,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D163" s="1">
         <v>0</v>
@@ -3095,7 +3175,7 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D164" s="1">
         <v>0</v>
@@ -3103,76 +3183,73 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>148</v>
+        <v>147</v>
+      </c>
+      <c r="C165" t="s">
+        <v>462</v>
       </c>
       <c r="D165" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D166" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>150</v>
-      </c>
       <c r="D167" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D168" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
-        <v>152</v>
-      </c>
       <c r="D169" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D170" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>151</v>
+      </c>
       <c r="D171" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D172" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
-        <v>155</v>
-      </c>
       <c r="D173" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D174" s="1">
         <v>0</v>
@@ -3180,23 +3257,20 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D175" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A176" t="s">
-        <v>158</v>
-      </c>
       <c r="D176" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D177" s="1">
         <v>0</v>
@@ -3204,7 +3278,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D178" s="1">
         <v>0</v>
@@ -3212,7 +3286,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D179" s="1">
         <v>0</v>
@@ -3220,7 +3294,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D180" s="1">
         <v>0</v>
@@ -3228,7 +3302,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D181" s="1">
         <v>0</v>
@@ -3236,7 +3310,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D182" s="1">
         <v>0</v>
@@ -3244,7 +3318,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D183" s="1">
         <v>0</v>
@@ -3252,7 +3326,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D184" s="1">
         <v>0</v>
@@ -3260,7 +3334,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D185" s="1">
         <v>0</v>
@@ -3268,7 +3342,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D186" s="1">
         <v>0</v>
@@ -3276,33 +3350,39 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D187" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>166</v>
+      </c>
       <c r="D188" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D189" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>168</v>
+      </c>
       <c r="D190" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D191" s="1">
         <v>0</v>
@@ -3310,7 +3390,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D192" s="1">
         <v>0</v>
@@ -3318,20 +3398,23 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D193" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>172</v>
+      </c>
       <c r="D194" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D195" s="1">
         <v>0</v>
@@ -3339,28 +3422,28 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
+        <v>174</v>
+      </c>
+      <c r="D196" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
         <v>175</v>
       </c>
-      <c r="D196" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D197" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A198" t="s">
-        <v>176</v>
-      </c>
       <c r="D198" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D199" s="1">
         <v>0</v>
@@ -3368,7 +3451,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D200" s="1">
         <v>0</v>
@@ -3376,7 +3459,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D201" s="1">
         <v>0</v>
@@ -3384,7 +3467,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D202" s="1">
         <v>0</v>
@@ -3392,7 +3475,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D203" s="1">
         <v>0</v>
@@ -3400,7 +3483,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D204" s="1">
         <v>0</v>
@@ -3408,7 +3491,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D205" s="1">
         <v>0</v>
@@ -3416,7 +3499,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D206" s="1">
         <v>0</v>
@@ -3424,7 +3507,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D207" s="1">
         <v>0</v>
@@ -3432,7 +3515,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D208" s="1">
         <v>0</v>
@@ -3440,7 +3523,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D209" s="1">
         <v>0</v>
@@ -3448,7 +3531,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D210" s="1">
         <v>0</v>
@@ -3456,7 +3539,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D211" s="1">
         <v>0</v>
@@ -3464,7 +3547,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D212" s="1">
         <v>0</v>
@@ -3472,23 +3555,20 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D213" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A214" t="s">
-        <v>192</v>
-      </c>
       <c r="D214" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D215" s="1">
         <v>0</v>
@@ -3496,7 +3576,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D216" s="1">
         <v>0</v>
@@ -3504,7 +3584,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D217" s="1">
         <v>0</v>
@@ -3512,20 +3592,23 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D218" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>195</v>
+      </c>
       <c r="D219" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D220" s="1">
         <v>0</v>
@@ -3533,7 +3616,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D221" s="1">
         <v>0</v>
@@ -3541,7 +3624,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D222" s="1">
         <v>0</v>
@@ -3549,7 +3632,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D223" s="1">
         <v>0</v>
@@ -3557,7 +3640,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D224" s="1">
         <v>0</v>
@@ -3565,7 +3648,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D225" s="1">
         <v>0</v>
@@ -3573,7 +3656,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D226" s="1">
         <v>0</v>
@@ -3581,7 +3664,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D227" s="1">
         <v>0</v>
@@ -3589,7 +3672,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D228" s="1">
         <v>0</v>
@@ -3597,7 +3680,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D229" s="1">
         <v>0</v>
@@ -3605,7 +3688,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D230" s="1">
         <v>0</v>
@@ -3613,7 +3696,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D231" s="1">
         <v>0</v>
@@ -3621,7 +3704,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D232" s="1">
         <v>0</v>
@@ -3629,28 +3712,28 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
+        <v>209</v>
+      </c>
+      <c r="D233" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D234" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
         <v>210</v>
       </c>
-      <c r="D233" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A234" t="s">
-        <v>211</v>
-      </c>
-      <c r="D234" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D235" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D236" s="1">
         <v>0</v>
@@ -3658,7 +3741,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D237" s="1">
         <v>0</v>
@@ -3666,148 +3749,145 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D238" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A239" t="s">
-        <v>215</v>
-      </c>
       <c r="D239" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
+        <v>214</v>
+      </c>
+      <c r="C240" t="s">
+        <v>465</v>
+      </c>
+      <c r="D240" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>215</v>
+      </c>
+      <c r="D241" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
         <v>216</v>
       </c>
-      <c r="D240" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A241" t="s">
+      <c r="D242" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
         <v>217</v>
       </c>
-      <c r="D241" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A242" t="s">
+      <c r="D243" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D244" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
         <v>218</v>
       </c>
-      <c r="D242" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A243" t="s">
+      <c r="D245" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
         <v>219</v>
       </c>
-      <c r="D243" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A244" t="s">
+      <c r="D246" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
         <v>220</v>
       </c>
-      <c r="D244" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A245" t="s">
+      <c r="D247" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D248" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
         <v>221</v>
       </c>
-      <c r="D245" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A246" t="s">
+      <c r="D249" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D250" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
         <v>222</v>
       </c>
-      <c r="D246" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A247" t="s">
+      <c r="D251" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
         <v>223</v>
       </c>
-      <c r="D247" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A248" t="s">
+      <c r="D252" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D253" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
         <v>224</v>
       </c>
-      <c r="D248" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A249" t="s">
+      <c r="C254" t="s">
+        <v>469</v>
+      </c>
+      <c r="D254" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E254" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
         <v>225</v>
       </c>
-      <c r="D249" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A250" t="s">
+      <c r="D255" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
         <v>226</v>
-      </c>
-      <c r="D250" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A251" t="s">
-        <v>227</v>
-      </c>
-      <c r="D251" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A252" t="s">
-        <v>228</v>
-      </c>
-      <c r="D252" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A253" t="s">
-        <v>229</v>
-      </c>
-      <c r="D253" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A254" t="s">
-        <v>230</v>
-      </c>
-      <c r="D254" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D255" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A256" t="s">
-        <v>231</v>
       </c>
       <c r="D256" s="1">
         <v>0</v>
@@ -3815,7 +3895,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D257" s="1">
         <v>0</v>
@@ -3823,7 +3903,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D258" s="1">
         <v>0</v>
@@ -3831,20 +3911,23 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D259" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>230</v>
+      </c>
       <c r="D260" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D261" s="1">
         <v>0</v>
@@ -3852,7 +3935,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D262" s="1">
         <v>0</v>
@@ -3860,7 +3943,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D263" s="1">
         <v>0</v>
@@ -3868,20 +3951,23 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D264" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>235</v>
+      </c>
       <c r="D265" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D266" s="1">
         <v>0</v>
@@ -3889,7 +3975,7 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D267" s="1">
         <v>0</v>
@@ -3897,33 +3983,39 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D268" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>239</v>
+      </c>
       <c r="D269" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D270" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>241</v>
+      </c>
       <c r="D271" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D272" s="1">
         <v>0</v>
@@ -3931,7 +4023,7 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D273" s="1">
         <v>0</v>
@@ -3944,7 +4036,7 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D275" s="1">
         <v>0</v>
@@ -3952,25 +4044,31 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
+        <v>245</v>
+      </c>
+      <c r="D276" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
         <v>246</v>
       </c>
-      <c r="D276" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D277" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>247</v>
+      </c>
       <c r="D278" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D279" s="1">
         <v>0</v>
@@ -3978,7 +4076,7 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D280" s="1">
         <v>0</v>
@@ -3986,7 +4084,7 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D281" s="1">
         <v>0</v>
@@ -3994,7 +4092,7 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D282" s="1">
         <v>0</v>
@@ -4002,7 +4100,7 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D283" s="1">
         <v>0</v>
@@ -4010,7 +4108,7 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D284" s="1">
         <v>0</v>
@@ -4018,7 +4116,7 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D285" s="1">
         <v>0</v>
@@ -4026,7 +4124,7 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D286" s="1">
         <v>0</v>
@@ -4034,7 +4132,7 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D287" s="1">
         <v>0</v>
@@ -4042,7 +4140,7 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D288" s="1">
         <v>0</v>
@@ -4050,7 +4148,7 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D289" s="1">
         <v>0</v>
@@ -4058,7 +4156,7 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D290" s="1">
         <v>0</v>
@@ -4066,7 +4164,7 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D291" s="1">
         <v>0</v>
@@ -4074,7 +4172,7 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D292" s="1">
         <v>0</v>
@@ -4082,7 +4180,7 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D293" s="1">
         <v>0</v>
@@ -4090,7 +4188,7 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D294" s="1">
         <v>0</v>
@@ -4098,7 +4196,7 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D295" s="1">
         <v>0</v>
@@ -4106,7 +4204,7 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D296" s="1">
         <v>0</v>
@@ -4114,7 +4212,7 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D297" s="1">
         <v>0</v>
@@ -4122,20 +4220,23 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D298" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A299" t="s">
+        <v>268</v>
+      </c>
       <c r="D299" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D300" s="1">
         <v>0</v>
@@ -4143,7 +4244,7 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D301" s="1">
         <v>0</v>
@@ -4151,7 +4252,7 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D302" s="1">
         <v>0</v>
@@ -4159,7 +4260,7 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D303" s="1">
         <v>0</v>
@@ -4167,7 +4268,7 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D304" s="1">
         <v>0</v>
@@ -4175,7 +4276,7 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D305" s="1">
         <v>0</v>
@@ -4183,7 +4284,7 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D306" s="1">
         <v>0</v>
@@ -4191,7 +4292,7 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D307" s="1">
         <v>0</v>
@@ -4199,7 +4300,7 @@
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D308" s="1">
         <v>0</v>
@@ -4207,7 +4308,7 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D309" s="1">
         <v>0</v>
@@ -4215,7 +4316,7 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D310" s="1">
         <v>0</v>
@@ -4223,7 +4324,7 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D311" s="1">
         <v>0</v>
@@ -4231,7 +4332,7 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D312" s="1">
         <v>0</v>
@@ -4239,7 +4340,7 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D313" s="1">
         <v>0</v>
@@ -4247,7 +4348,7 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D314" s="1">
         <v>0</v>
@@ -4255,7 +4356,7 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D315" s="1">
         <v>0</v>
@@ -4263,7 +4364,7 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D316" s="1">
         <v>0</v>
@@ -4271,7 +4372,7 @@
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D317" s="1">
         <v>0</v>
@@ -4279,7 +4380,7 @@
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D318" s="1">
         <v>0</v>
@@ -4287,7 +4388,7 @@
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D319" s="1">
         <v>0</v>
@@ -4295,7 +4396,7 @@
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D320" s="1">
         <v>0</v>
@@ -4303,7 +4404,7 @@
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D321" s="1">
         <v>0</v>
@@ -4311,7 +4412,7 @@
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D322" s="1">
         <v>0</v>
@@ -4319,7 +4420,7 @@
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D323" s="1">
         <v>0</v>
@@ -4327,7 +4428,7 @@
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D324" s="1">
         <v>0</v>
@@ -4335,7 +4436,7 @@
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D325" s="1">
         <v>0</v>
@@ -4343,7 +4444,7 @@
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D326" s="1">
         <v>0</v>
@@ -4351,7 +4452,7 @@
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D327" s="1">
         <v>0</v>
@@ -4359,7 +4460,7 @@
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D328" s="1">
         <v>0</v>
@@ -4367,7 +4468,7 @@
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D329" s="1">
         <v>0</v>
@@ -4375,7 +4476,7 @@
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D330" s="1">
         <v>0</v>
@@ -4383,7 +4484,7 @@
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D331" s="1">
         <v>0</v>
@@ -4391,7 +4492,7 @@
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D332" s="1">
         <v>0</v>
@@ -4399,7 +4500,7 @@
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D333" s="1">
         <v>0</v>
@@ -4407,7 +4508,7 @@
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D334" s="1">
         <v>0</v>
@@ -4415,7 +4516,7 @@
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D335" s="1">
         <v>0</v>
@@ -4423,7 +4524,7 @@
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D336" s="1">
         <v>0</v>
@@ -4431,7 +4532,7 @@
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D337" s="1">
         <v>0</v>
@@ -4439,7 +4540,7 @@
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D338" s="1">
         <v>0</v>
@@ -4447,7 +4548,7 @@
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D339" s="1">
         <v>0</v>
@@ -4455,7 +4556,7 @@
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D340" s="1">
         <v>0</v>
@@ -4463,7 +4564,7 @@
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D341" s="1">
         <v>0</v>
@@ -4471,7 +4572,7 @@
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D342" s="1">
         <v>0</v>
@@ -4479,7 +4580,7 @@
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D343" s="1">
         <v>0</v>
@@ -4487,7 +4588,7 @@
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D344" s="1">
         <v>0</v>
@@ -4495,7 +4596,7 @@
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D345" s="1">
         <v>0</v>
@@ -4503,7 +4604,7 @@
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D346" s="1">
         <v>0</v>
@@ -4511,7 +4612,7 @@
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D347" s="1">
         <v>0</v>
@@ -4519,7 +4620,7 @@
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D348" s="1">
         <v>0</v>
@@ -4527,7 +4628,7 @@
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D349" s="1">
         <v>0</v>
@@ -4535,7 +4636,7 @@
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D350" s="1">
         <v>0</v>
@@ -4543,7 +4644,7 @@
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D351" s="1">
         <v>0</v>
@@ -4551,7 +4652,7 @@
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D352" s="1">
         <v>0</v>
@@ -4559,7 +4660,7 @@
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D353" s="1">
         <v>0</v>
@@ -4567,7 +4668,7 @@
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D354" s="1">
         <v>0</v>
@@ -4575,7 +4676,7 @@
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D355" s="1">
         <v>0</v>
@@ -4583,7 +4684,7 @@
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D356" s="1">
         <v>0</v>
@@ -4591,7 +4692,7 @@
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D357" s="1">
         <v>0</v>
@@ -4599,7 +4700,7 @@
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D358" s="1">
         <v>0</v>
@@ -4607,7 +4708,7 @@
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D359" s="1">
         <v>0</v>
@@ -4615,7 +4716,7 @@
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D360" s="1">
         <v>0</v>
@@ -4623,7 +4724,7 @@
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D361" s="1">
         <v>0</v>
@@ -4631,7 +4732,7 @@
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D362" s="1">
         <v>0</v>
@@ -4639,7 +4740,7 @@
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D363" s="1">
         <v>0</v>
@@ -4647,7 +4748,7 @@
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D364" s="1">
         <v>0</v>
@@ -4655,7 +4756,7 @@
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="D365" s="1">
         <v>0</v>
@@ -4663,7 +4764,7 @@
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D366" s="1">
         <v>0</v>
@@ -4671,7 +4772,7 @@
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D367" s="1">
         <v>0</v>
@@ -4679,7 +4780,7 @@
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D368" s="1">
         <v>0</v>
@@ -4687,7 +4788,7 @@
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D369" s="1">
         <v>0</v>
@@ -4695,7 +4796,7 @@
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D370" s="1">
         <v>0</v>
@@ -4703,7 +4804,7 @@
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D371" s="1">
         <v>0</v>
@@ -4711,7 +4812,7 @@
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D372" s="1">
         <v>0</v>
@@ -4719,7 +4820,7 @@
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D373" s="1">
         <v>0</v>
@@ -4727,7 +4828,7 @@
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D374" s="1">
         <v>0</v>
@@ -4735,7 +4836,7 @@
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D375" s="1">
         <v>0</v>
@@ -4743,7 +4844,7 @@
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D376" s="1">
         <v>0</v>
@@ -4751,7 +4852,7 @@
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D377" s="1">
         <v>0</v>
@@ -4759,7 +4860,7 @@
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D378" s="1">
         <v>0</v>
@@ -4767,7 +4868,7 @@
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D379" s="1">
         <v>0</v>
@@ -4775,7 +4876,7 @@
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D380" s="1">
         <v>0</v>
@@ -4783,7 +4884,7 @@
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D381" s="1">
         <v>0</v>
@@ -4791,7 +4892,7 @@
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D382" s="1">
         <v>0</v>
@@ -4799,7 +4900,7 @@
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D383" s="1">
         <v>0</v>
@@ -4807,7 +4908,7 @@
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D384" s="1">
         <v>0</v>
@@ -4815,7 +4916,7 @@
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D385" s="1">
         <v>0</v>
@@ -4823,7 +4924,7 @@
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D386" s="1">
         <v>0</v>
@@ -4831,7 +4932,7 @@
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D387" s="1">
         <v>0</v>
@@ -4839,7 +4940,7 @@
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D388" s="1">
         <v>0</v>
@@ -4847,7 +4948,7 @@
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D389" s="1">
         <v>0</v>
@@ -4855,7 +4956,7 @@
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D390" s="1">
         <v>0</v>
@@ -4863,7 +4964,7 @@
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D391" s="1">
         <v>0</v>
@@ -4871,7 +4972,7 @@
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D392" s="1">
         <v>0</v>
@@ -4879,7 +4980,7 @@
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D393" s="1">
         <v>0</v>
@@ -4887,7 +4988,7 @@
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="D394" s="1">
         <v>0</v>
@@ -4895,7 +4996,7 @@
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D395" s="1">
         <v>0</v>
@@ -4903,7 +5004,7 @@
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D396" s="1">
         <v>0</v>
@@ -4911,7 +5012,7 @@
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D397" s="1">
         <v>0</v>
@@ -4919,7 +5020,7 @@
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D398" s="1">
         <v>0</v>
@@ -4927,7 +5028,7 @@
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D399" s="1">
         <v>0</v>
@@ -4935,7 +5036,7 @@
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="D400" s="1">
         <v>0</v>
@@ -4943,7 +5044,7 @@
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D401" s="1">
         <v>0</v>
@@ -4951,7 +5052,7 @@
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D402" s="1">
         <v>0</v>
@@ -4959,7 +5060,7 @@
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D403" s="1">
         <v>0</v>
@@ -4967,7 +5068,7 @@
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D404" s="1">
         <v>0</v>
@@ -4975,7 +5076,7 @@
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="D405" s="1">
         <v>0</v>
@@ -4983,7 +5084,7 @@
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D406" s="1">
         <v>0</v>
@@ -4991,7 +5092,7 @@
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D407" s="1">
         <v>0</v>
@@ -4999,7 +5100,7 @@
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D408" s="1">
         <v>0</v>
@@ -5007,7 +5108,7 @@
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D409" s="1">
         <v>0</v>
@@ -5015,7 +5116,7 @@
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="D410" s="1">
         <v>0</v>
@@ -5023,7 +5124,7 @@
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="D411" s="1">
         <v>0</v>
@@ -5031,7 +5132,7 @@
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D412" s="1">
         <v>0</v>
@@ -5039,7 +5140,7 @@
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D413" s="1">
         <v>0</v>
@@ -5047,7 +5148,7 @@
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="D414" s="1">
         <v>0</v>
@@ -5055,7 +5156,7 @@
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="D415" s="1">
         <v>0</v>
@@ -5063,7 +5164,7 @@
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D416" s="1">
         <v>0</v>
@@ -5071,7 +5172,7 @@
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D417" s="1">
         <v>0</v>
@@ -5079,7 +5180,7 @@
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D418" s="1">
         <v>0</v>
@@ -5087,7 +5188,7 @@
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D419" s="1">
         <v>0</v>
@@ -5095,7 +5196,7 @@
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="D420" s="1">
         <v>0</v>
@@ -5103,7 +5204,7 @@
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="D421" s="1">
         <v>0</v>
@@ -5111,7 +5212,7 @@
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="D422" s="1">
         <v>0</v>
@@ -5119,7 +5220,7 @@
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D423" s="1">
         <v>0</v>
@@ -5127,7 +5228,7 @@
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D424" s="1">
         <v>0</v>
@@ -5135,7 +5236,7 @@
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="D425" s="1">
         <v>0</v>
@@ -5143,7 +5244,7 @@
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D426" s="1">
         <v>0</v>
@@ -5151,7 +5252,7 @@
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D427" s="1">
         <v>0</v>
@@ -5159,7 +5260,7 @@
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="D428" s="1">
         <v>0</v>
@@ -5167,7 +5268,7 @@
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="D429" s="1">
         <v>0</v>
@@ -5175,7 +5276,7 @@
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="D430" s="1">
         <v>0</v>
@@ -5183,7 +5284,7 @@
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="D431" s="1">
         <v>0</v>
@@ -5191,7 +5292,7 @@
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="D432" s="1">
         <v>0</v>
@@ -5199,7 +5300,7 @@
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="D433" s="1">
         <v>0</v>
@@ -5207,7 +5308,7 @@
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="D434" s="1">
         <v>0</v>
@@ -5215,7 +5316,7 @@
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D435" s="1">
         <v>0</v>
@@ -5223,7 +5324,7 @@
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D436" s="1">
         <v>0</v>
@@ -5231,7 +5332,7 @@
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="D437" s="1">
         <v>0</v>
@@ -5239,7 +5340,7 @@
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D438" s="1">
         <v>0</v>
@@ -5247,7 +5348,7 @@
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="D439" s="1">
         <v>0</v>
@@ -5255,7 +5356,7 @@
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="D440" s="1">
         <v>0</v>
@@ -5263,7 +5364,7 @@
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="D441" s="1">
         <v>0</v>
@@ -5271,7 +5372,7 @@
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="D442" s="1">
         <v>0</v>
@@ -5279,7 +5380,7 @@
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="D443" s="1">
         <v>0</v>
@@ -5287,7 +5388,7 @@
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D444" s="1">
         <v>0</v>
@@ -5295,7 +5396,7 @@
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D445" s="1">
         <v>0</v>
@@ -5303,7 +5404,7 @@
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D446" s="1">
         <v>0</v>
@@ -5311,7 +5412,7 @@
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="D447" s="1">
         <v>0</v>
@@ -5319,7 +5420,7 @@
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="D448" s="1">
         <v>0</v>
@@ -5327,7 +5428,7 @@
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D449" s="1">
         <v>0</v>
@@ -5335,7 +5436,7 @@
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D450" s="1">
         <v>0</v>
@@ -5343,7 +5444,7 @@
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D451" s="1">
         <v>0</v>
@@ -5351,7 +5452,7 @@
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D452" s="1">
         <v>0</v>
@@ -5359,7 +5460,7 @@
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="D453" s="1">
         <v>0</v>
@@ -5367,7 +5468,7 @@
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D454" s="1">
         <v>0</v>
@@ -5375,7 +5476,7 @@
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="D455" s="1">
         <v>0</v>
@@ -5383,7 +5484,7 @@
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D456" s="1">
         <v>0</v>
@@ -5391,7 +5492,7 @@
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="D457" s="1">
         <v>0</v>
@@ -5399,7 +5500,7 @@
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D458" s="1">
         <v>0</v>
@@ -5407,7 +5508,7 @@
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="D459" s="1">
         <v>0</v>
@@ -5415,7 +5516,7 @@
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A460" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="D460" s="1">
         <v>0</v>
@@ -5423,7 +5524,7 @@
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D461" s="1">
         <v>0</v>
@@ -5431,7 +5532,7 @@
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="D462" s="1">
         <v>0</v>
@@ -5439,7 +5540,7 @@
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="D463" s="1">
         <v>0</v>
@@ -5447,7 +5548,7 @@
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="D464" s="1">
         <v>0</v>
@@ -5455,7 +5556,7 @@
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="D465" s="1">
         <v>0</v>
@@ -5463,7 +5564,7 @@
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D466" s="1">
         <v>0</v>
@@ -5471,7 +5572,7 @@
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D467" s="1">
         <v>0</v>
@@ -5479,7 +5580,7 @@
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="D468" s="1">
         <v>0</v>
@@ -5487,7 +5588,7 @@
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="D469" s="1">
         <v>0</v>
@@ -5495,7 +5596,7 @@
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D470" s="1">
         <v>0</v>
@@ -5503,7 +5604,7 @@
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="D471" s="1">
         <v>0</v>
@@ -5511,7 +5612,7 @@
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D472" s="1">
         <v>0</v>
@@ -5519,7 +5620,7 @@
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A473" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="D473" s="1">
         <v>0</v>
@@ -5527,209 +5628,9 @@
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D474" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="475" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A475" t="s">
-        <v>442</v>
-      </c>
-      <c r="D475" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="476" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A476" t="s">
-        <v>443</v>
-      </c>
-      <c r="D476" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="477" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A477" t="s">
-        <v>444</v>
-      </c>
-      <c r="D477" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="478" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A478" t="s">
-        <v>445</v>
-      </c>
-      <c r="D478" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="479" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A479" t="s">
-        <v>446</v>
-      </c>
-      <c r="D479" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="480" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A480" t="s">
-        <v>447</v>
-      </c>
-      <c r="D480" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="481" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A481" t="s">
-        <v>448</v>
-      </c>
-      <c r="D481" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="482" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A482" t="s">
-        <v>449</v>
-      </c>
-      <c r="D482" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="483" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A483" t="s">
-        <v>450</v>
-      </c>
-      <c r="D483" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="484" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A484" t="s">
-        <v>451</v>
-      </c>
-      <c r="D484" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="485" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A485" t="s">
-        <v>452</v>
-      </c>
-      <c r="D485" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="486" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A486" t="s">
-        <v>453</v>
-      </c>
-      <c r="D486" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="487" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A487" t="s">
-        <v>454</v>
-      </c>
-      <c r="D487" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="488" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A488" t="s">
-        <v>455</v>
-      </c>
-      <c r="D488" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="489" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A489" t="s">
-        <v>456</v>
-      </c>
-      <c r="D489" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="490" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A490" t="s">
-        <v>457</v>
-      </c>
-      <c r="D490" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="491" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A491" t="s">
-        <v>458</v>
-      </c>
-      <c r="D491" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="492" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A492" t="s">
-        <v>459</v>
-      </c>
-      <c r="D492" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="493" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A493" t="s">
-        <v>460</v>
-      </c>
-      <c r="D493" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="494" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A494" t="s">
-        <v>461</v>
-      </c>
-      <c r="D494" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="495" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A495" t="s">
-        <v>462</v>
-      </c>
-      <c r="D495" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="496" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A496" t="s">
-        <v>463</v>
-      </c>
-      <c r="D496" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="497" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A497" t="s">
-        <v>464</v>
-      </c>
-      <c r="D497" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="498" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A498" t="s">
-        <v>465</v>
-      </c>
-      <c r="D498" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="499" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A499" t="s">
-        <v>466</v>
-      </c>
-      <c r="D499" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>